<commit_message>
Fix minor error of excel parsing
</commit_message>
<xml_diff>
--- a/definition/xlsx/SLCO1B1_allele_definition_table.xlsx
+++ b/definition/xlsx/SLCO1B1_allele_definition_table.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jing/work/pharmacogenomics/PharmGKB/allele_definition_table_1_12_19/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CD921BF-6354-C04C-B14F-F3519403481D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="2040" windowWidth="28800" windowHeight="16480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alleles" sheetId="1" r:id="rId1"/>
     <sheet name="Change log" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -550,7 +556,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -751,7 +757,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -929,12 +935,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1170,7 +1170,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1221,25 +1221,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="96">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1638,17 +1619,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="10" topLeftCell="U11" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="23.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.83203125" style="3" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="13.83203125" style="3" customWidth="1" collapsed="1"/>
@@ -1656,7 +1634,7 @@
     <col min="4" max="4" width="14.1640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="12" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="12.5" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.1640625" style="25" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11.5" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="11.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="11.5" style="3" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1672,7 +1650,7 @@
     <col min="22" max="22" width="13" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="13.6640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="25" width="13" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="12" style="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="27" max="27" width="12.5" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="13" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="29" max="29" width="14.1640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1681,7 +1659,7 @@
     <col min="40" max="16384" width="23.33203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>74</v>
       </c>
@@ -1690,7 +1668,7 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
-      <c r="G1" s="22"/>
+      <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -1709,13 +1687,13 @@
       <c r="W1" s="7"/>
       <c r="X1" s="7"/>
       <c r="Y1" s="7"/>
-      <c r="Z1" s="22"/>
+      <c r="Z1" s="7"/>
       <c r="AA1" s="7"/>
       <c r="AB1" s="7"/>
       <c r="AC1" s="7"/>
       <c r="AD1" s="7"/>
     </row>
-    <row r="2" spans="1:30" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="2" spans="1:30" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>170</v>
       </c>
@@ -1734,7 +1712,7 @@
       <c r="F2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="1" t="s">
         <v>94</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1791,7 +1769,7 @@
       <c r="Y2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Z2" s="23" t="s">
+      <c r="Z2" s="1" t="s">
         <v>148</v>
       </c>
       <c r="AA2" s="1" t="s">
@@ -1807,7 +1785,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="40" customHeight="1">
+    <row r="3" spans="1:30" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>168</v>
       </c>
@@ -1824,7 +1802,7 @@
       <c r="F3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="1" t="s">
         <v>94</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1881,7 +1859,7 @@
       <c r="Y3" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Z3" s="23" t="s">
+      <c r="Z3" s="1" t="s">
         <v>148</v>
       </c>
       <c r="AA3" s="1" t="s">
@@ -1897,7 +1875,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="67" customHeight="1">
+    <row r="4" spans="1:30" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>77</v>
       </c>
@@ -1916,7 +1894,7 @@
       <c r="F4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="1" t="s">
         <v>93</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1973,7 +1951,7 @@
       <c r="Y4" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="Z4" s="23" t="s">
+      <c r="Z4" s="1" t="s">
         <v>147</v>
       </c>
       <c r="AA4" s="1" t="s">
@@ -1989,7 +1967,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="59" customHeight="1">
+    <row r="5" spans="1:30" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>76</v>
       </c>
@@ -2008,7 +1986,7 @@
       <c r="F5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -2065,7 +2043,7 @@
       <c r="Y5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="Z5" s="23" t="s">
+      <c r="Z5" s="1" t="s">
         <v>146</v>
       </c>
       <c r="AA5" s="1" t="s">
@@ -2081,7 +2059,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="18" customHeight="1">
+    <row r="6" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>75</v>
       </c>
@@ -2100,7 +2078,7 @@
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -2155,7 +2133,7 @@
       <c r="Y6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Z6" s="23" t="s">
+      <c r="Z6" s="1" t="s">
         <v>53</v>
       </c>
       <c r="AA6" s="1" t="s">
@@ -2171,7 +2149,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="36" customHeight="1">
+    <row r="7" spans="1:30" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -2180,7 +2158,7 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="24"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -2199,13 +2177,13 @@
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
-      <c r="Z7" s="24"/>
+      <c r="Z7" s="10"/>
       <c r="AA7" s="10"/>
       <c r="AB7" s="10"/>
       <c r="AC7" s="10"/>
       <c r="AD7" s="10"/>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -2224,7 +2202,7 @@
       <c r="F8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -2281,7 +2259,7 @@
       <c r="Y8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Z8" s="23" t="s">
+      <c r="Z8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="AA8" s="1" t="s">
@@ -2297,7 +2275,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2306,7 +2284,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H9" s="1"/>
@@ -2327,13 +2305,13 @@
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="23"/>
+      <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -2344,7 +2322,7 @@
         <v>55</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2363,13 +2341,13 @@
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
-      <c r="Z10" s="23"/>
+      <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -2380,7 +2358,7 @@
       <c r="F11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="23"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -2401,13 +2379,13 @@
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="23"/>
+      <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -2416,7 +2394,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="23"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
@@ -2437,13 +2415,13 @@
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="23"/>
+      <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2452,7 +2430,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="23"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -2473,13 +2451,13 @@
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
-      <c r="Z13" s="23"/>
+      <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -2488,7 +2466,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="23"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -2509,13 +2487,13 @@
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="23"/>
+      <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -2524,7 +2502,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="23"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2545,13 +2523,13 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
-      <c r="Z15" s="23"/>
+      <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -2560,7 +2538,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -2581,13 +2559,13 @@
         <v>54</v>
       </c>
       <c r="Y16" s="1"/>
-      <c r="Z16" s="23"/>
+      <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -2596,7 +2574,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2617,13 +2595,13 @@
       <c r="Y17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z17" s="23"/>
+      <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -2632,7 +2610,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="23"/>
+      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2651,7 +2629,7 @@
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
-      <c r="Z18" s="23"/>
+      <c r="Z18" s="1"/>
       <c r="AA18" s="1" t="s">
         <v>54</v>
       </c>
@@ -2659,7 +2637,7 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2668,7 +2646,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2687,7 +2665,7 @@
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
-      <c r="Z19" s="23"/>
+      <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1" t="s">
         <v>54</v>
@@ -2695,7 +2673,7 @@
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2706,7 +2684,7 @@
         <v>55</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2725,7 +2703,7 @@
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
-      <c r="Z20" s="23"/>
+      <c r="Z20" s="1"/>
       <c r="AA20" s="1" t="s">
         <v>54</v>
       </c>
@@ -2733,7 +2711,7 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -2744,7 +2722,7 @@
       <c r="F21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="23"/>
+      <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2765,7 +2743,7 @@
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
-      <c r="Z21" s="23"/>
+      <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1" t="s">
         <v>54</v>
@@ -2773,7 +2751,7 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -2782,7 +2760,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H22" s="1"/>
@@ -2805,13 +2783,13 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
-      <c r="Z22" s="23"/>
+      <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -2820,7 +2798,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H23" s="1"/>
@@ -2843,13 +2821,13 @@
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
-      <c r="Z23" s="23"/>
+      <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -2858,7 +2836,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="23"/>
+      <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
         <v>16</v>
@@ -2879,13 +2857,13 @@
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
-      <c r="Z24" s="23"/>
+      <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -2896,7 +2874,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="23" t="s">
+      <c r="G25" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H25" s="1"/>
@@ -2919,13 +2897,13 @@
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
-      <c r="Z25" s="23"/>
+      <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
@@ -2934,7 +2912,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="23" t="s">
+      <c r="G26" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -2963,13 +2941,13 @@
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
-      <c r="Z26" s="23"/>
+      <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
@@ -2978,7 +2956,7 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="23"/>
+      <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -2999,7 +2977,7 @@
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
-      <c r="Z27" s="23" t="s">
+      <c r="Z27" s="1" t="s">
         <v>55</v>
       </c>
       <c r="AA27" s="1"/>
@@ -3007,7 +2985,7 @@
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>70</v>
       </c>
@@ -3016,7 +2994,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="23" t="s">
+      <c r="G28" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H28" s="1"/>
@@ -3039,7 +3017,7 @@
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
-      <c r="Z28" s="23" t="s">
+      <c r="Z28" s="1" t="s">
         <v>55</v>
       </c>
       <c r="AA28" s="1"/>
@@ -3047,7 +3025,7 @@
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>71</v>
       </c>
@@ -3058,7 +3036,7 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="23" t="s">
+      <c r="G29" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H29" s="1"/>
@@ -3081,13 +3059,13 @@
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
-      <c r="Z29" s="23"/>
+      <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -3096,7 +3074,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="23"/>
+      <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -3115,7 +3093,7 @@
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
-      <c r="Z30" s="23" t="s">
+      <c r="Z30" s="1" t="s">
         <v>55</v>
       </c>
       <c r="AA30" s="1"/>
@@ -3123,7 +3101,7 @@
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -3134,7 +3112,7 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="23"/>
+      <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -3153,13 +3131,13 @@
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
-      <c r="Z31" s="23"/>
+      <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -3168,7 +3146,7 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="23" t="s">
+      <c r="G32" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H32" s="1"/>
@@ -3191,13 +3169,13 @@
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
-      <c r="Z32" s="23"/>
+      <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="1:30">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
@@ -3206,7 +3184,7 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="23" t="s">
+      <c r="G33" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H33" s="1"/>
@@ -3233,13 +3211,13 @@
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="1"/>
-      <c r="Z33" s="23"/>
+      <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -3248,7 +3226,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="23"/>
+      <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -3269,13 +3247,13 @@
       </c>
       <c r="X34" s="1"/>
       <c r="Y34" s="1"/>
-      <c r="Z34" s="23"/>
+      <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -3284,7 +3262,7 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="23" t="s">
+      <c r="G35" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H35" s="1"/>
@@ -3307,13 +3285,13 @@
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
-      <c r="Z35" s="23"/>
+      <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -3322,7 +3300,7 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="23" t="s">
+      <c r="G36" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H36" s="1"/>
@@ -3347,13 +3325,13 @@
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
       <c r="Y36" s="1"/>
-      <c r="Z36" s="23"/>
+      <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -3362,7 +3340,7 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="23" t="s">
+      <c r="G37" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H37" s="1"/>
@@ -3383,7 +3361,7 @@
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
       <c r="Y37" s="1"/>
-      <c r="Z37" s="23"/>
+      <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
@@ -3391,7 +3369,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:30">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -3400,7 +3378,7 @@
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="23" t="s">
+      <c r="G38" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H38" s="1"/>
@@ -3423,13 +3401,13 @@
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
       <c r="Y38" s="1"/>
-      <c r="Z38" s="23"/>
+      <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
     </row>
-    <row r="39" spans="1:30">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -3438,7 +3416,7 @@
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="23" t="s">
+      <c r="G39" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H39" s="1"/>
@@ -3461,13 +3439,13 @@
       <c r="Y39" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z39" s="23"/>
+      <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
     </row>
-    <row r="40" spans="1:30">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -3476,7 +3454,7 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="23" t="s">
+      <c r="G40" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H40" s="1"/>
@@ -3501,13 +3479,13 @@
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
-      <c r="Z40" s="23"/>
+      <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" spans="1:30">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -3518,7 +3496,7 @@
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="23" t="s">
+      <c r="G41" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H41" s="1"/>
@@ -3543,13 +3521,13 @@
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
-      <c r="Z41" s="23"/>
+      <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" spans="1:30">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -3558,7 +3536,7 @@
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="23"/>
+      <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -3577,7 +3555,7 @@
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
-      <c r="Z42" s="23"/>
+      <c r="Z42" s="1"/>
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
       <c r="AC42" s="1" t="s">
@@ -3585,7 +3563,7 @@
       </c>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="1:30">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -3594,7 +3572,7 @@
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="23" t="s">
+      <c r="G43" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H43" s="1"/>
@@ -3615,7 +3593,7 @@
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
-      <c r="Z43" s="23" t="s">
+      <c r="Z43" s="1" t="s">
         <v>55</v>
       </c>
       <c r="AA43" s="1"/>
@@ -3623,7 +3601,7 @@
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" spans="1:30">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -3632,7 +3610,7 @@
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="23"/>
+      <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -3653,49 +3631,41 @@
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
-      <c r="Z44" s="23"/>
+      <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
     </row>
-    <row r="46" spans="1:30" ht="15">
+    <row r="46" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:30" s="14" customFormat="1" ht="15">
+    <row r="47" spans="1:30" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="G47" s="26"/>
-      <c r="Z47" s="26"/>
-    </row>
-    <row r="48" spans="1:30" s="14" customFormat="1" ht="15">
+    </row>
+    <row r="48" spans="1:30" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="G48" s="26"/>
-      <c r="Z48" s="26"/>
-    </row>
-    <row r="49" spans="1:26" s="17" customFormat="1" ht="15">
+    </row>
+    <row r="49" spans="1:1" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="G49" s="27"/>
-      <c r="Z49" s="27"/>
-    </row>
-    <row r="50" spans="1:26" s="15" customFormat="1" ht="15">
+    </row>
+    <row r="50" spans="1:1" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="G50" s="28"/>
-      <c r="Z50" s="28"/>
-    </row>
-    <row r="51" spans="1:26">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="11"/>
     </row>
-    <row r="52" spans="1:26">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="11"/>
     </row>
   </sheetData>
@@ -3710,19 +3680,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB9BE5B-A704-C94E-BB24-3AA159BE7168}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="20" customFormat="1">
+    <row r="1" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>172</v>
       </c>
@@ -3730,12 +3700,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="21">
         <v>43213</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="21">
         <v>43746</v>
       </c>
@@ -3745,10 +3715,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>